<commit_message>
Updated the masterdata file to cover 1950-2014, now includes coverage
</commit_message>
<xml_diff>
--- a/searches/bayes.xlsx
+++ b/searches/bayes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="139">
   <si>
     <t>#</t>
   </si>
@@ -339,6 +339,108 @@
   </si>
   <si>
     <t>PY 1997 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>PY 1998 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>PY 1999 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>PY 2000 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>PY 2001 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>PY 2002 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>PY 2003 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>PY 2004 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>PY 2005 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>PY 2006 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>PY 2007 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>PY 2008 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>PY 2009 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>PY 2010 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>PY 2011 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>PY 2012 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>PY 2013 AND PT Peer Reviewed Journal AND AB bayes*</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>PY 2014 AND PT Peer Reviewed Journal AND AB bayes*</t>
   </si>
 </sst>
 </file>
@@ -473,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -486,6 +588,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -506,6 +614,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -788,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D142" sqref="A1:E145"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143:E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,1687 +937,2526 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="8"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
       <c r="D34" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
       <c r="D39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
       <c r="D40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
       <c r="D42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
       <c r="D43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="8"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
       <c r="D45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="8"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
       <c r="D46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="8"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
       <c r="D48" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="8"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
       <c r="D49" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E49" s="8"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E50" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
       <c r="D51" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E51" s="8"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
       <c r="D52" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="10"/>
     </row>
     <row r="53" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
       <c r="D54" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
       <c r="D55" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="8"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="10">
         <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
+      <c r="A57" s="8"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
       <c r="D57" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E57" s="8"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
       <c r="D58" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E58" s="8"/>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59" s="10">
         <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
       <c r="D60" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E60" s="8"/>
+      <c r="E60" s="10"/>
     </row>
     <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
+      <c r="A61" s="8"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
       <c r="D61" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E61" s="8"/>
+      <c r="E61" s="10"/>
     </row>
     <row r="62" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E62" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
+      <c r="A63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
       <c r="D63" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E63" s="8"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
       <c r="D64" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E64" s="8"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E65" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
+      <c r="A66" s="8"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
       <c r="D66" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E66" s="8"/>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
+      <c r="A67" s="8"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
       <c r="D67" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E67" s="8"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E68" s="8">
+      <c r="E68" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
+      <c r="A69" s="8"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
       <c r="D69" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="8"/>
+      <c r="E69" s="10"/>
     </row>
     <row r="70" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
       <c r="D70" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="8"/>
+      <c r="E70" s="10"/>
     </row>
     <row r="71" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C71" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E71" s="8">
+      <c r="E71" s="10">
         <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
+      <c r="A72" s="8"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
       <c r="D72" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E72" s="8"/>
+      <c r="E72" s="10"/>
     </row>
     <row r="73" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
+      <c r="A73" s="8"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
       <c r="D73" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="8"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E74" s="8">
+      <c r="E74" s="10">
         <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
+      <c r="A75" s="8"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
       <c r="D75" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E75" s="8"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A76" s="6"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
+      <c r="A76" s="8"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
       <c r="D76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E76" s="8"/>
+      <c r="E76" s="10"/>
     </row>
     <row r="77" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B77" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E77" s="8">
+      <c r="E77" s="10">
         <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A78" s="6"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
+      <c r="A78" s="8"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
       <c r="D78" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E78" s="8"/>
+      <c r="E78" s="10"/>
     </row>
     <row r="79" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
+      <c r="A79" s="8"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
       <c r="D79" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E79" s="8"/>
+      <c r="E79" s="10"/>
     </row>
     <row r="80" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E80" s="8">
+      <c r="E80" s="10">
         <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
+      <c r="A81" s="8"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
       <c r="D81" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E81" s="8"/>
+      <c r="E81" s="10"/>
     </row>
     <row r="82" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
       <c r="D82" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E82" s="8"/>
+      <c r="E82" s="10"/>
     </row>
     <row r="83" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B83" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C83" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E83" s="8">
+      <c r="E83" s="10">
         <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9"/>
       <c r="D84" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E84" s="8"/>
+      <c r="E84" s="10"/>
     </row>
     <row r="85" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A85" s="6"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
+      <c r="A85" s="8"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
       <c r="D85" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E85" s="8"/>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B86" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E86" s="8">
+      <c r="E86" s="10">
         <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A87" s="6"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
+      <c r="A87" s="8"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="9"/>
       <c r="D87" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E87" s="8"/>
+      <c r="E87" s="10"/>
     </row>
     <row r="88" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="9"/>
       <c r="D88" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E88" s="8"/>
+      <c r="E88" s="10"/>
     </row>
     <row r="89" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="B89" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E89" s="8">
+      <c r="E89" s="10">
         <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A90" s="6"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9"/>
       <c r="D90" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E90" s="8"/>
+      <c r="E90" s="10"/>
     </row>
     <row r="91" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A91" s="6"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
+      <c r="A91" s="8"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="9"/>
       <c r="D91" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E91" s="8"/>
+      <c r="E91" s="10"/>
     </row>
     <row r="92" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B92" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C92" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E92" s="8">
+      <c r="E92" s="10">
         <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A93" s="6"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
+      <c r="A93" s="8"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="9"/>
       <c r="D93" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E93" s="8"/>
+      <c r="E93" s="10"/>
     </row>
     <row r="94" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A94" s="6"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="9"/>
       <c r="D94" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E94" s="8"/>
+      <c r="E94" s="10"/>
     </row>
     <row r="95" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
+      <c r="A95" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B95" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E95" s="8">
+      <c r="E95" s="10">
         <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A96" s="6"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
       <c r="D96" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E96" s="8"/>
+      <c r="E96" s="10"/>
     </row>
     <row r="97" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A97" s="6"/>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
+      <c r="A97" s="8"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
       <c r="D97" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E97" s="8"/>
+      <c r="E97" s="10"/>
     </row>
     <row r="98" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
+      <c r="A98" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B98" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C98" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E98" s="8">
+      <c r="E98" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A99" s="6"/>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
+      <c r="A99" s="8"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9"/>
       <c r="D99" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E99" s="8"/>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A100" s="6"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
+      <c r="A100" s="8"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="9"/>
       <c r="D100" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E100" s="8"/>
+      <c r="E100" s="10"/>
     </row>
     <row r="101" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B101" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C101" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E101" s="8">
+      <c r="E101" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A102" s="6"/>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
+      <c r="A102" s="8"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="9"/>
       <c r="D102" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E102" s="8"/>
+      <c r="E102" s="10"/>
     </row>
     <row r="103" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A103" s="6"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="7"/>
+      <c r="A103" s="8"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="9"/>
       <c r="D103" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E103" s="8"/>
+      <c r="E103" s="10"/>
     </row>
     <row r="104" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B104" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E104" s="8">
+      <c r="E104" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A105" s="6"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
+      <c r="A105" s="8"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="9"/>
       <c r="D105" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E105" s="8"/>
+      <c r="E105" s="10"/>
     </row>
     <row r="106" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
+      <c r="A106" s="8"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="9"/>
       <c r="D106" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E106" s="8"/>
+      <c r="E106" s="10"/>
     </row>
     <row r="107" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="6" t="s">
+      <c r="A107" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B107" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E107" s="8">
+      <c r="E107" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A108" s="6"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
+      <c r="A108" s="8"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="9"/>
       <c r="D108" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E108" s="8"/>
+      <c r="E108" s="10"/>
     </row>
     <row r="109" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A109" s="6"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
+      <c r="A109" s="8"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="9"/>
       <c r="D109" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E109" s="8"/>
+      <c r="E109" s="10"/>
     </row>
     <row r="110" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="6" t="s">
+      <c r="A110" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B110" s="7" t="s">
+      <c r="B110" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C110" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E110" s="8">
+      <c r="E110" s="10">
         <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A111" s="6"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
+      <c r="A111" s="8"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="9"/>
       <c r="D111" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E111" s="8"/>
+      <c r="E111" s="10"/>
     </row>
     <row r="112" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A112" s="6"/>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
+      <c r="A112" s="8"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
       <c r="D112" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E112" s="8"/>
+      <c r="E112" s="10"/>
     </row>
     <row r="113" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="6" t="s">
+      <c r="A113" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B113" s="7" t="s">
+      <c r="B113" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C113" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E113" s="8">
+      <c r="E113" s="10">
         <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A114" s="6"/>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
+      <c r="A114" s="8"/>
+      <c r="B114" s="9"/>
+      <c r="C114" s="9"/>
       <c r="D114" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E114" s="8"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A115" s="6"/>
-      <c r="B115" s="7"/>
-      <c r="C115" s="7"/>
+      <c r="A115" s="8"/>
+      <c r="B115" s="9"/>
+      <c r="C115" s="9"/>
       <c r="D115" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E115" s="8"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="6" t="s">
+      <c r="A116" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B116" s="7" t="s">
+      <c r="B116" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C116" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E116" s="8">
+      <c r="E116" s="10">
         <v>26</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A117" s="6"/>
-      <c r="B117" s="7"/>
-      <c r="C117" s="7"/>
+      <c r="A117" s="8"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="9"/>
       <c r="D117" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E117" s="8"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A118" s="6"/>
-      <c r="B118" s="7"/>
-      <c r="C118" s="7"/>
+      <c r="A118" s="8"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
       <c r="D118" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E118" s="8"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B119" s="7" t="s">
+      <c r="B119" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E119" s="8">
+      <c r="E119" s="10">
         <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A120" s="6"/>
-      <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
+      <c r="A120" s="8"/>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
       <c r="D120" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E120" s="8"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A121" s="6"/>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
+      <c r="A121" s="8"/>
+      <c r="B121" s="9"/>
+      <c r="C121" s="9"/>
       <c r="D121" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E121" s="8"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="6" t="s">
+      <c r="A122" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B122" s="7" t="s">
+      <c r="B122" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="C122" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E122" s="8">
+      <c r="E122" s="10">
         <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A123" s="6"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
+      <c r="A123" s="8"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="9"/>
       <c r="D123" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E123" s="8"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A124" s="6"/>
-      <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
+      <c r="A124" s="8"/>
+      <c r="B124" s="9"/>
+      <c r="C124" s="9"/>
       <c r="D124" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E124" s="8"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="6" t="s">
+      <c r="A125" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B125" s="7" t="s">
+      <c r="B125" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C125" s="7" t="s">
+      <c r="C125" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E125" s="8">
+      <c r="E125" s="10">
         <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A126" s="6"/>
-      <c r="B126" s="7"/>
-      <c r="C126" s="7"/>
+      <c r="A126" s="8"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="9"/>
       <c r="D126" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E126" s="8"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A127" s="6"/>
-      <c r="B127" s="7"/>
-      <c r="C127" s="7"/>
+      <c r="A127" s="8"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="9"/>
       <c r="D127" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E127" s="8"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="B128" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C128" s="7" t="s">
+      <c r="C128" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E128" s="8">
+      <c r="E128" s="10">
         <v>32</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A129" s="6"/>
-      <c r="B129" s="7"/>
-      <c r="C129" s="7"/>
+      <c r="A129" s="8"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="9"/>
       <c r="D129" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E129" s="8"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A130" s="6"/>
-      <c r="B130" s="7"/>
-      <c r="C130" s="7"/>
+      <c r="A130" s="8"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="9"/>
       <c r="D130" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E130" s="8"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B131" s="7" t="s">
+      <c r="B131" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C131" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E131" s="8">
+      <c r="E131" s="10">
         <v>21</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A132" s="6"/>
-      <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
+      <c r="A132" s="8"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="9"/>
       <c r="D132" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E132" s="8"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A133" s="6"/>
-      <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
+      <c r="A133" s="8"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="9"/>
       <c r="D133" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E133" s="8"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="6" t="s">
+      <c r="A134" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B134" s="7" t="s">
+      <c r="B134" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C134" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E134" s="8">
+      <c r="E134" s="10">
         <v>23</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A135" s="6"/>
-      <c r="B135" s="7"/>
-      <c r="C135" s="7"/>
+      <c r="A135" s="8"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="9"/>
       <c r="D135" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E135" s="8"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A136" s="6"/>
-      <c r="B136" s="7"/>
-      <c r="C136" s="7"/>
+      <c r="A136" s="8"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="9"/>
       <c r="D136" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E136" s="8"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B137" s="7" t="s">
+      <c r="B137" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C137" s="7" t="s">
+      <c r="C137" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E137" s="8">
+      <c r="E137" s="10">
         <v>46</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A138" s="6"/>
-      <c r="B138" s="7"/>
-      <c r="C138" s="7"/>
+      <c r="A138" s="8"/>
+      <c r="B138" s="9"/>
+      <c r="C138" s="9"/>
       <c r="D138" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E138" s="8"/>
+      <c r="E138" s="10"/>
     </row>
     <row r="139" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A139" s="6"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
+      <c r="A139" s="8"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="9"/>
       <c r="D139" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E139" s="8"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="B140" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C140" s="7" t="s">
+      <c r="C140" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E140" s="8">
+      <c r="E140" s="10">
         <v>52</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A141" s="6"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="7"/>
+      <c r="A141" s="8"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
       <c r="D141" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E141" s="8"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A142" s="6"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="7"/>
+      <c r="A142" s="8"/>
+      <c r="B142" s="9"/>
+      <c r="C142" s="9"/>
       <c r="D142" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E142" s="8"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B143" s="7" t="s">
+      <c r="B143" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C143" s="7" t="s">
+      <c r="C143" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E143" s="8">
+      <c r="E143" s="10">
         <v>61</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="48" x14ac:dyDescent="0.25">
-      <c r="A144" s="6"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
+      <c r="A144" s="8"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="9"/>
       <c r="D144" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E144" s="8"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="9"/>
-      <c r="B145" s="10"/>
-      <c r="C145" s="10"/>
+      <c r="A145" s="11"/>
+      <c r="B145" s="12"/>
+      <c r="C145" s="12"/>
       <c r="D145" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E145" s="11"/>
+      <c r="E145" s="13"/>
+    </row>
+    <row r="146" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A146" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C146" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D146" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E146" s="18">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A147" s="8"/>
+      <c r="B147" s="17"/>
+      <c r="C147" s="17"/>
+      <c r="D147" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E147" s="10"/>
+    </row>
+    <row r="148" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A148" s="8"/>
+      <c r="B148" s="17"/>
+      <c r="C148" s="17"/>
+      <c r="D148" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E148" s="10"/>
+    </row>
+    <row r="149" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A149" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D149" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E149" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A150" s="8"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E150" s="10"/>
+    </row>
+    <row r="151" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A151" s="8"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E151" s="10"/>
+    </row>
+    <row r="152" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A152" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E152" s="10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A153" s="8"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E153" s="10"/>
+    </row>
+    <row r="154" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A154" s="8"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E154" s="10"/>
+    </row>
+    <row r="155" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A155" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D155" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E155" s="10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A156" s="8"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E156" s="10"/>
+    </row>
+    <row r="157" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A157" s="8"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E157" s="10"/>
+    </row>
+    <row r="158" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A158" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E158" s="10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A159" s="8"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E159" s="10"/>
+    </row>
+    <row r="160" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A160" s="8"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="9"/>
+      <c r="D160" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E160" s="10"/>
+    </row>
+    <row r="161" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A161" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D161" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E161" s="10">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A162" s="8"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E162" s="10"/>
+    </row>
+    <row r="163" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A163" s="8"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E163" s="10"/>
+    </row>
+    <row r="164" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A164" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C164" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D164" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E164" s="10">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A165" s="8"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E165" s="10"/>
+    </row>
+    <row r="166" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A166" s="8"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="9"/>
+      <c r="D166" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E166" s="10"/>
+    </row>
+    <row r="167" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A167" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E167" s="10">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A168" s="8"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="9"/>
+      <c r="D168" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E168" s="10"/>
+    </row>
+    <row r="169" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A169" s="8"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E169" s="10"/>
+    </row>
+    <row r="170" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A170" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D170" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E170" s="10">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A171" s="8"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E171" s="10"/>
+    </row>
+    <row r="172" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A172" s="8"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E172" s="10"/>
+    </row>
+    <row r="173" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A173" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B173" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C173" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D173" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E173" s="10">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A174" s="8"/>
+      <c r="B174" s="9"/>
+      <c r="C174" s="9"/>
+      <c r="D174" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E174" s="10"/>
+    </row>
+    <row r="175" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A175" s="8"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E175" s="10"/>
+    </row>
+    <row r="176" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A176" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B176" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D176" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E176" s="10">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A177" s="8"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="9"/>
+      <c r="D177" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E177" s="10"/>
+    </row>
+    <row r="178" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A178" s="8"/>
+      <c r="B178" s="9"/>
+      <c r="C178" s="9"/>
+      <c r="D178" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E178" s="10"/>
+    </row>
+    <row r="179" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A179" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B179" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D179" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E179" s="10">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A180" s="8"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="9"/>
+      <c r="D180" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E180" s="10"/>
+    </row>
+    <row r="181" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A181" s="8"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E181" s="10"/>
+    </row>
+    <row r="182" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A182" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B182" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C182" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D182" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E182" s="10">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A183" s="8"/>
+      <c r="B183" s="9"/>
+      <c r="C183" s="9"/>
+      <c r="D183" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E183" s="10"/>
+    </row>
+    <row r="184" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A184" s="8"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E184" s="10"/>
+    </row>
+    <row r="185" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A185" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B185" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D185" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E185" s="10">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A186" s="8"/>
+      <c r="B186" s="9"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E186" s="10"/>
+    </row>
+    <row r="187" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A187" s="8"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E187" s="10"/>
+    </row>
+    <row r="188" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A188" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B188" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D188" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E188" s="10">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A189" s="8"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="9"/>
+      <c r="D189" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E189" s="10"/>
+    </row>
+    <row r="190" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A190" s="8"/>
+      <c r="B190" s="9"/>
+      <c r="C190" s="9"/>
+      <c r="D190" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E190" s="10"/>
+    </row>
+    <row r="191" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A191" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B191" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D191" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E191" s="10">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A192" s="8"/>
+      <c r="B192" s="9"/>
+      <c r="C192" s="9"/>
+      <c r="D192" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E192" s="10"/>
+    </row>
+    <row r="193" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A193" s="8"/>
+      <c r="B193" s="9"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E193" s="10"/>
+    </row>
+    <row r="194" spans="1:5" ht="72" x14ac:dyDescent="0.25">
+      <c r="A194" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B194" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D194" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E194" s="10">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="48" x14ac:dyDescent="0.25">
+      <c r="A195" s="8"/>
+      <c r="B195" s="9"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E195" s="10"/>
+    </row>
+    <row r="196" spans="1:5" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="11"/>
+      <c r="B196" s="12"/>
+      <c r="C196" s="12"/>
+      <c r="D196" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E196" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="192">
+  <mergeCells count="260">
+    <mergeCell ref="A191:A193"/>
+    <mergeCell ref="B191:B193"/>
+    <mergeCell ref="C191:C193"/>
+    <mergeCell ref="E191:E193"/>
+    <mergeCell ref="A194:A196"/>
+    <mergeCell ref="B194:B196"/>
+    <mergeCell ref="C194:C196"/>
+    <mergeCell ref="E194:E196"/>
+    <mergeCell ref="A182:A184"/>
+    <mergeCell ref="B182:B184"/>
+    <mergeCell ref="C182:C184"/>
+    <mergeCell ref="E182:E184"/>
+    <mergeCell ref="A185:A187"/>
+    <mergeCell ref="B185:B187"/>
+    <mergeCell ref="C185:C187"/>
+    <mergeCell ref="E185:E187"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="B188:B190"/>
+    <mergeCell ref="C188:C190"/>
+    <mergeCell ref="E188:E190"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="C173:C175"/>
+    <mergeCell ref="E173:E175"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="B176:B178"/>
+    <mergeCell ref="C176:C178"/>
+    <mergeCell ref="E176:E178"/>
+    <mergeCell ref="A179:A181"/>
+    <mergeCell ref="B179:B181"/>
+    <mergeCell ref="C179:C181"/>
+    <mergeCell ref="E179:E181"/>
+    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="C164:C166"/>
+    <mergeCell ref="E164:E166"/>
+    <mergeCell ref="A167:A169"/>
+    <mergeCell ref="B167:B169"/>
+    <mergeCell ref="C167:C169"/>
+    <mergeCell ref="E167:E169"/>
+    <mergeCell ref="A170:A172"/>
+    <mergeCell ref="B170:B172"/>
+    <mergeCell ref="C170:C172"/>
+    <mergeCell ref="E170:E172"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="B155:B157"/>
+    <mergeCell ref="C155:C157"/>
+    <mergeCell ref="E155:E157"/>
+    <mergeCell ref="A158:A160"/>
+    <mergeCell ref="B158:B160"/>
+    <mergeCell ref="C158:C160"/>
+    <mergeCell ref="E158:E160"/>
+    <mergeCell ref="A161:A163"/>
+    <mergeCell ref="B161:B163"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="E161:E163"/>
+    <mergeCell ref="A146:A148"/>
+    <mergeCell ref="B146:B148"/>
+    <mergeCell ref="C146:C148"/>
+    <mergeCell ref="E146:E148"/>
+    <mergeCell ref="A149:A151"/>
+    <mergeCell ref="B149:B151"/>
+    <mergeCell ref="C149:C151"/>
+    <mergeCell ref="E149:E151"/>
+    <mergeCell ref="A152:A154"/>
+    <mergeCell ref="B152:B154"/>
+    <mergeCell ref="C152:C154"/>
+    <mergeCell ref="E152:E154"/>
+    <mergeCell ref="A140:A142"/>
+    <mergeCell ref="B140:B142"/>
+    <mergeCell ref="E140:E142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="E143:E145"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="E134:E136"/>
+    <mergeCell ref="A137:A139"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="E137:E139"/>
+    <mergeCell ref="C134:C136"/>
+    <mergeCell ref="C137:C139"/>
+    <mergeCell ref="C140:C142"/>
+    <mergeCell ref="C143:C145"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="E128:E130"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="E131:E133"/>
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="E122:E124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="E125:E127"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="C128:C130"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="E116:E118"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="E119:E121"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="E104:E106"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="B107:B109"/>
+    <mergeCell ref="E107:E109"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="E98:E100"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="E101:E103"/>
+    <mergeCell ref="C98:C100"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="C107:C109"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="E92:E94"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="E95:E97"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="C95:C97"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="E80:E82"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="E83:E85"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B77:B79"/>
+    <mergeCell ref="E77:E79"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="C80:C82"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="E71:E73"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="C68:C70"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="E8:E10"/>
@@ -2511,182 +3473,6 @@
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="E80:E82"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="E83:E85"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B77:B79"/>
-    <mergeCell ref="E77:E79"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="C80:C82"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="E92:E94"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="E95:E97"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="E89:E91"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="C95:C97"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="E104:E106"/>
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="B107:B109"/>
-    <mergeCell ref="E107:E109"/>
-    <mergeCell ref="A98:A100"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="E98:E100"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="E101:E103"/>
-    <mergeCell ref="C98:C100"/>
-    <mergeCell ref="C101:C103"/>
-    <mergeCell ref="C104:C106"/>
-    <mergeCell ref="C107:C109"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="E116:E118"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="E119:E121"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="C119:C121"/>
-    <mergeCell ref="A128:A130"/>
-    <mergeCell ref="B128:B130"/>
-    <mergeCell ref="E128:E130"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="B131:B133"/>
-    <mergeCell ref="E131:E133"/>
-    <mergeCell ref="A122:A124"/>
-    <mergeCell ref="B122:B124"/>
-    <mergeCell ref="E122:E124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="E125:E127"/>
-    <mergeCell ref="C122:C124"/>
-    <mergeCell ref="C125:C127"/>
-    <mergeCell ref="C128:C130"/>
-    <mergeCell ref="C131:C133"/>
-    <mergeCell ref="A140:A142"/>
-    <mergeCell ref="B140:B142"/>
-    <mergeCell ref="E140:E142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="B143:B145"/>
-    <mergeCell ref="E143:E145"/>
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="E134:E136"/>
-    <mergeCell ref="A137:A139"/>
-    <mergeCell ref="B137:B139"/>
-    <mergeCell ref="E137:E139"/>
-    <mergeCell ref="C134:C136"/>
-    <mergeCell ref="C137:C139"/>
-    <mergeCell ref="C140:C142"/>
-    <mergeCell ref="C143:C145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>